<commit_message>
initiation for excel now works - should be applied to maininitiation though
</commit_message>
<xml_diff>
--- a/Feriekasse.xlsx
+++ b/Feriekasse.xlsx
@@ -413,14 +413,299 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Kim</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Point</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Emil</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Point</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Mads</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Point</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Soren</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Point</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Chelsea</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Dortmund</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Ac Milan</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Fc midtjylland</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Atalanta</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>FC Kbenhavn</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>sevilla</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>RB Leipzig</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Real sociedad</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Frankfurt</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>juventus</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>AGF</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Tottenham</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Arsenal</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Manchester Utd</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Bologna</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Brndby IF</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Valencia</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Leverkusen</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>OB</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Leicester</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Hoffenheim</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Torino</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Total:</t>
+        </is>
+      </c>
+      <c r="B8">
+        <f>SUM(B2:B7)</f>
+        <v/>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Total:</t>
+        </is>
+      </c>
+      <c r="D8">
+        <f>SUM(D2:D7)</f>
+        <v/>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Total:</t>
+        </is>
+      </c>
+      <c r="F8">
+        <f>SUM(F2:F7)</f>
+        <v/>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Total:</t>
+        </is>
+      </c>
+      <c r="H8">
+        <f>SUM(H2:H7)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
done with fixing master
</commit_message>
<xml_diff>
--- a/Feriekasse.xlsx
+++ b/Feriekasse.xlsx
@@ -424,42 +424,46 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t xml:space="preserve">Kim
+</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Point</t>
+          <t>Point:</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Emil</t>
+          <t xml:space="preserve">Emil
+</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Point</t>
+          <t>Point:</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>Mads</t>
+          <t xml:space="preserve">Mads
+</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>Point</t>
+          <t>Point:</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>Soren</t>
+          <t xml:space="preserve">Soren
+</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>Point</t>
+          <t>Point:</t>
         </is>
       </c>
     </row>
@@ -474,7 +478,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Leicester</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -482,7 +486,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Ac Milan</t>
+          <t>Arsenal</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -490,7 +494,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Fc midtjylland</t>
+          <t>Manchester utd</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -500,7 +504,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Barcelona</t>
+          <t>RB leipzig</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -508,7 +512,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Atalanta</t>
+          <t>Tottenham</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -516,7 +520,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>FC Kbenhavn</t>
+          <t>Frankfurt</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -524,7 +528,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>sevilla</t>
+          <t>Leverkusen</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -534,7 +538,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -542,7 +546,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Real sociedad</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -550,7 +554,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Frankfurt</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -558,7 +562,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>juventus</t>
+          <t>sevilla</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -568,7 +572,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AGF</t>
+          <t>Bologna</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -576,7 +580,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Tottenham</t>
+          <t>Real sociedad</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -584,7 +588,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Arsenal</t>
+          <t>Valencia</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -592,7 +596,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Manchester Utd</t>
+          <t>juventus</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -602,7 +606,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Bologna</t>
+          <t>OB</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -610,7 +614,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Brndby IF</t>
+          <t>Atalanta</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -618,7 +622,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Valencia</t>
+          <t>Ac Milan</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -626,7 +630,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Leverkusen</t>
+          <t>Torino</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -636,7 +640,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>AGF</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -644,7 +648,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Leicester</t>
+          <t>Brndby IF</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -652,7 +656,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>FC Kbenhavn</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -660,7 +664,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Torino</t>
+          <t>FC midtjylland</t>
         </is>
       </c>
       <c r="H7" t="n">

</xml_diff>

<commit_message>
minor bugfixes for excel, added outline for updating excel
</commit_message>
<xml_diff>
--- a/Feriekasse.xlsx
+++ b/Feriekasse.xlsx
@@ -494,7 +494,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Manchester utd</t>
+          <t>Man Utd</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -648,7 +648,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Brndby IF</t>
+          <t>Brndby</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -656,7 +656,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>FC Kbenhavn</t>
+          <t>FCK</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -664,7 +664,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>FC midtjylland</t>
+          <t>FC Midtjylland</t>
         </is>
       </c>
       <c r="H7" t="n">

</xml_diff>

<commit_message>
orjson does not work for latest match covered i think
</commit_message>
<xml_diff>
--- a/Feriekasse.xlsx
+++ b/Feriekasse.xlsx
@@ -424,8 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Kim
-</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -435,8 +434,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Emil
-</t>
+          <t>Emil</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -446,8 +444,7 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Mads
-</t>
+          <t>Mads</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
@@ -457,8 +454,7 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t xml:space="preserve">Soren
-</t>
+          <t>Soren</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
@@ -473,66 +469,74 @@
           <t>Chelsea</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
+      <c r="B2">
+        <f>0</f>
+        <v/>
       </c>
       <c r="C2" t="inlineStr">
         <is>
           <t>Leicester</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>0</v>
+      <c r="D2">
+        <f>0</f>
+        <v/>
       </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>Arsenal</t>
         </is>
       </c>
-      <c r="F2" t="n">
-        <v>0</v>
+      <c r="F2">
+        <f>0</f>
+        <v/>
       </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>Man Utd</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>0</v>
+      <c r="H2">
+        <f>0</f>
+        <v/>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RB leipzig</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>0</v>
+          <t>RB Leipzig</t>
+        </is>
+      </c>
+      <c r="B3">
+        <f>0</f>
+        <v/>
       </c>
       <c r="C3" t="inlineStr">
         <is>
           <t>Tottenham</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
+      <c r="D3">
+        <f>0</f>
+        <v/>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Frankfurt</t>
-        </is>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
+          <t>Eintracht Frankfurt</t>
+        </is>
+      </c>
+      <c r="F3">
+        <f>0</f>
+        <v/>
       </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>Leverkusen</t>
         </is>
       </c>
-      <c r="H3" t="n">
-        <v>0</v>
+      <c r="H3">
+        <f>0</f>
+        <v/>
       </c>
     </row>
     <row r="4">
@@ -541,32 +545,36 @@
           <t>Barcelona</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0</v>
+      <c r="B4">
+        <f>0</f>
+        <v/>
       </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>Dortmund</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>0</v>
+      <c r="D4">
+        <f>0</f>
+        <v/>
       </c>
       <c r="E4" t="inlineStr">
         <is>
           <t>Hoffenheim</t>
         </is>
       </c>
-      <c r="F4" t="n">
-        <v>0</v>
+      <c r="F4">
+        <f>0</f>
+        <v/>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>sevilla</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>0</v>
+          <t>Sevilla</t>
+        </is>
+      </c>
+      <c r="H4">
+        <f>0</f>
+        <v/>
       </c>
     </row>
     <row r="5">
@@ -575,32 +583,36 @@
           <t>Bologna</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>0</v>
+      <c r="B5">
+        <f>0</f>
+        <v/>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Real sociedad</t>
-        </is>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
+          <t>Real Sociedad</t>
+        </is>
+      </c>
+      <c r="D5">
+        <f>0</f>
+        <v/>
       </c>
       <c r="E5" t="inlineStr">
         <is>
           <t>Valencia</t>
         </is>
       </c>
-      <c r="F5" t="n">
-        <v>0</v>
+      <c r="F5">
+        <f>0</f>
+        <v/>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>juventus</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>0</v>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="H5">
+        <f>0</f>
+        <v/>
       </c>
     </row>
     <row r="6">
@@ -609,32 +621,36 @@
           <t>OB</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>0</v>
+      <c r="B6">
+        <f>0</f>
+        <v/>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>Atalanta</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>0</v>
+      <c r="D6">
+        <f>0</f>
+        <v/>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Ac Milan</t>
-        </is>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
+          <t>Milan</t>
+        </is>
+      </c>
+      <c r="F6">
+        <f>0</f>
+        <v/>
       </c>
       <c r="G6" t="inlineStr">
         <is>
           <t>Torino</t>
         </is>
       </c>
-      <c r="H6" t="n">
-        <v>0</v>
+      <c r="H6">
+        <f>0</f>
+        <v/>
       </c>
     </row>
     <row r="7">
@@ -643,32 +659,36 @@
           <t>AGF</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>0</v>
+      <c r="B7">
+        <f>0</f>
+        <v/>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Brndby</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
+          <t>Brøndby</t>
+        </is>
+      </c>
+      <c r="D7">
+        <f>0</f>
+        <v/>
       </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>FCK</t>
         </is>
       </c>
-      <c r="F7" t="n">
-        <v>0</v>
+      <c r="F7">
+        <f>0</f>
+        <v/>
       </c>
       <c r="G7" t="inlineStr">
         <is>
           <t>FC Midtjylland</t>
         </is>
       </c>
-      <c r="H7" t="n">
-        <v>0</v>
+      <c r="H7">
+        <f>0</f>
+        <v/>
       </c>
     </row>
     <row r="8">

</xml_diff>

<commit_message>
Done with menu - still need to implement boundary so you cant start mid game
</commit_message>
<xml_diff>
--- a/Feriekasse.xlsx
+++ b/Feriekasse.xlsx
@@ -424,37 +424,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Søren</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Point:</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Mads</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Point:</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>Kim</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Point:</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Emil</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Point:</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Mads</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Point:</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Soren</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
@@ -475,7 +475,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Leicester</t>
+          <t>Liverpool</t>
         </is>
       </c>
       <c r="D2">
@@ -493,7 +493,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Man Utd</t>
+          <t>Man City</t>
         </is>
       </c>
       <c r="H2">
@@ -504,7 +504,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>RB Leipzig</t>
+          <t>Tottenham</t>
         </is>
       </c>
       <c r="B3">
@@ -513,7 +513,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Tottenham</t>
+          <t>Bayern</t>
         </is>
       </c>
       <c r="D3">
@@ -522,7 +522,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="F3">
@@ -542,7 +542,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Barcelona</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="B4">
@@ -551,7 +551,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="D4">
@@ -560,7 +560,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>1. FC Köln</t>
         </is>
       </c>
       <c r="F4">
@@ -569,7 +569,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Sevilla</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="H4">
@@ -580,7 +580,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bologna</t>
+          <t>Atlético Madrid</t>
         </is>
       </c>
       <c r="B5">
@@ -589,7 +589,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Real Sociedad</t>
+          <t>Sevilla</t>
         </is>
       </c>
       <c r="D5">
@@ -598,7 +598,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Valencia</t>
+          <t>Barcelona</t>
         </is>
       </c>
       <c r="F5">
@@ -607,7 +607,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Juventus</t>
+          <t>Real Madrid</t>
         </is>
       </c>
       <c r="H5">
@@ -618,7 +618,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>OB</t>
+          <t>Inter</t>
         </is>
       </c>
       <c r="B6">
@@ -627,7 +627,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Atalanta</t>
+          <t>Napoli</t>
         </is>
       </c>
       <c r="D6">
@@ -636,16 +636,16 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="F6">
+        <f>0</f>
+        <v/>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
           <t>Milan</t>
-        </is>
-      </c>
-      <c r="F6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Torino</t>
         </is>
       </c>
       <c r="H6">
@@ -656,7 +656,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AGF</t>
+          <t>Brøndby</t>
         </is>
       </c>
       <c r="B7">
@@ -665,7 +665,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Brøndby</t>
+          <t>FC Midtjylland</t>
         </is>
       </c>
       <c r="D7">
@@ -683,7 +683,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>FC Midtjylland</t>
+          <t>AaB</t>
         </is>
       </c>
       <c r="H7">

</xml_diff>

<commit_message>
it actually works now. mangler bare tests og cleanup
</commit_message>
<xml_diff>
--- a/Feriekasse.xlsx
+++ b/Feriekasse.xlsx
@@ -413,323 +413,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Søren</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Point:</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Mads</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>Point:</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Kim</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Point:</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Emil</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Point:</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Chelsea</t>
-        </is>
-      </c>
-      <c r="B2">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Liverpool</t>
-        </is>
-      </c>
-      <c r="D2">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Arsenal</t>
-        </is>
-      </c>
-      <c r="F2">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Man City</t>
-        </is>
-      </c>
-      <c r="H2">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Tottenham</t>
-        </is>
-      </c>
-      <c r="B3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Bayern</t>
-        </is>
-      </c>
-      <c r="D3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Dortmund</t>
-        </is>
-      </c>
-      <c r="F3">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Leverkusen</t>
-        </is>
-      </c>
-      <c r="H3">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Freiburg</t>
-        </is>
-      </c>
-      <c r="B4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Union Berlin</t>
-        </is>
-      </c>
-      <c r="D4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>1. FC Köln</t>
-        </is>
-      </c>
-      <c r="F4">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>RB Leipzig</t>
-        </is>
-      </c>
-      <c r="H4">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Atlético Madrid</t>
-        </is>
-      </c>
-      <c r="B5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Sevilla</t>
-        </is>
-      </c>
-      <c r="D5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Barcelona</t>
-        </is>
-      </c>
-      <c r="F5">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Real Madrid</t>
-        </is>
-      </c>
-      <c r="H5">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Inter</t>
-        </is>
-      </c>
-      <c r="B6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Napoli</t>
-        </is>
-      </c>
-      <c r="D6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Juventus</t>
-        </is>
-      </c>
-      <c r="F6">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Milan</t>
-        </is>
-      </c>
-      <c r="H6">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Brøndby</t>
-        </is>
-      </c>
-      <c r="B7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>FC Midtjylland</t>
-        </is>
-      </c>
-      <c r="D7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>FCK</t>
-        </is>
-      </c>
-      <c r="F7">
-        <f>0</f>
-        <v/>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>AaB</t>
-        </is>
-      </c>
-      <c r="H7">
-        <f>0</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Total:</t>
-        </is>
-      </c>
-      <c r="B8">
-        <f>SUM(B2:B7)</f>
-        <v/>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Total:</t>
-        </is>
-      </c>
-      <c r="D8">
-        <f>SUM(D2:D7)</f>
-        <v/>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Total:</t>
-        </is>
-      </c>
-      <c r="F8">
-        <f>SUM(F2:F7)</f>
-        <v/>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>Total:</t>
-        </is>
-      </c>
-      <c r="H8">
-        <f>SUM(H2:H7)</f>
-        <v/>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>